<commit_message>
update ZEV and LCFS policies; remove temp market share limits on biofuels
</commit_message>
<xml_diff>
--- a/csv/model/CIMS_market share limits/formula_CIMS_market share limits_AB.xlsx
+++ b/csv/model/CIMS_market share limits/formula_CIMS_market share limits_AB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\xCIMS\cims-models\csv\model\CIMS_market share limits\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AB97D3FD-8EBC-4CC6-B307-044D5C56F740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D6967127-8BAC-436C-B817-3C41F8788AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1800" windowWidth="51840" windowHeight="21120" xr2:uid="{62A98192-B4FE-4E2D-AB6B-B0684DBA4DB5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F2360103-3943-4AE6-85A5-A537BF27A022}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1261,21 +1261,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8188689E-71E8-4C01-8BB7-08510254719E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91B9294D-5427-4233-9F9E-F15DF0F78323}">
   <dimension ref="A1:X216"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:X216"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1349,7 +1349,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1408,7 +1408,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -1526,7 +1526,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1585,7 +1585,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1644,7 +1644,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -1762,7 +1762,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -1821,7 +1821,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -1880,7 +1880,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -1939,7 +1939,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -1998,7 +1998,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -2116,7 +2116,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -2175,7 +2175,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -2234,7 +2234,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -2293,7 +2293,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -2352,7 +2352,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>45</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>47</v>
       </c>
@@ -2470,7 +2470,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>48</v>
       </c>
@@ -2529,7 +2529,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -2588,7 +2588,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>54</v>
       </c>
@@ -2647,7 +2647,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>57</v>
       </c>
@@ -2706,7 +2706,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>60</v>
       </c>
@@ -2765,7 +2765,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>63</v>
       </c>
@@ -2824,7 +2824,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>63</v>
       </c>
@@ -2883,7 +2883,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>63</v>
       </c>
@@ -2942,7 +2942,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>68</v>
       </c>
@@ -3001,7 +3001,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>68</v>
       </c>
@@ -3060,7 +3060,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>68</v>
       </c>
@@ -3119,7 +3119,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>68</v>
       </c>
@@ -3178,7 +3178,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>73</v>
       </c>
@@ -3237,7 +3237,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>73</v>
       </c>
@@ -3296,7 +3296,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>78</v>
       </c>
@@ -3355,7 +3355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>81</v>
       </c>
@@ -3414,7 +3414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>84</v>
       </c>
@@ -3473,7 +3473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>84</v>
       </c>
@@ -3532,7 +3532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>89</v>
       </c>
@@ -3591,7 +3591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>89</v>
       </c>
@@ -3650,7 +3650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>93</v>
       </c>
@@ -3709,7 +3709,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>96</v>
       </c>
@@ -3768,7 +3768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>96</v>
       </c>
@@ -3827,7 +3827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>100</v>
       </c>
@@ -3886,7 +3886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>103</v>
       </c>
@@ -3945,7 +3945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>106</v>
       </c>
@@ -4004,7 +4004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>106</v>
       </c>
@@ -4063,7 +4063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>109</v>
       </c>
@@ -4122,7 +4122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>109</v>
       </c>
@@ -4181,7 +4181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>111</v>
       </c>
@@ -4240,7 +4240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>111</v>
       </c>
@@ -4299,7 +4299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>115</v>
       </c>
@@ -4358,7 +4358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>116</v>
       </c>
@@ -4417,7 +4417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>116</v>
       </c>
@@ -4476,7 +4476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>120</v>
       </c>
@@ -4535,7 +4535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>121</v>
       </c>
@@ -4594,7 +4594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>125</v>
       </c>
@@ -4653,7 +4653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>127</v>
       </c>
@@ -4712,7 +4712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>128</v>
       </c>
@@ -4771,7 +4771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>131</v>
       </c>
@@ -4830,7 +4830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>131</v>
       </c>
@@ -4889,7 +4889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>134</v>
       </c>
@@ -4948,7 +4948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>134</v>
       </c>
@@ -5007,7 +5007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>135</v>
       </c>
@@ -5066,7 +5066,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>135</v>
       </c>
@@ -5125,7 +5125,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>135</v>
       </c>
@@ -5184,7 +5184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>135</v>
       </c>
@@ -5243,7 +5243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>138</v>
       </c>
@@ -5302,7 +5302,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>140</v>
       </c>
@@ -5361,7 +5361,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>140</v>
       </c>
@@ -5420,7 +5420,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>140</v>
       </c>
@@ -5479,7 +5479,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>140</v>
       </c>
@@ -5538,7 +5538,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>142</v>
       </c>
@@ -5597,7 +5597,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>142</v>
       </c>
@@ -5656,7 +5656,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="76" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>142</v>
       </c>
@@ -5715,7 +5715,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="77" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>143</v>
       </c>
@@ -5774,7 +5774,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="78" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>143</v>
       </c>
@@ -5833,7 +5833,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="79" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>143</v>
       </c>
@@ -5892,7 +5892,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="80" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>144</v>
       </c>
@@ -5951,7 +5951,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="81" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>145</v>
       </c>
@@ -6010,7 +6010,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="82" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>146</v>
       </c>
@@ -6069,7 +6069,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="83" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>147</v>
       </c>
@@ -6128,7 +6128,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="84" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>148</v>
       </c>
@@ -6187,7 +6187,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="85" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>149</v>
       </c>
@@ -6246,7 +6246,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="86" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>150</v>
       </c>
@@ -6305,7 +6305,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="87" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>151</v>
       </c>
@@ -6364,7 +6364,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="88" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>152</v>
       </c>
@@ -6423,7 +6423,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="89" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>153</v>
       </c>
@@ -6482,7 +6482,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="90" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>153</v>
       </c>
@@ -6541,7 +6541,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="91" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>153</v>
       </c>
@@ -6600,7 +6600,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>153</v>
       </c>
@@ -6659,7 +6659,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="93" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>156</v>
       </c>
@@ -6718,7 +6718,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="94" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>156</v>
       </c>
@@ -6777,7 +6777,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="95" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>156</v>
       </c>
@@ -6836,7 +6836,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>156</v>
       </c>
@@ -6895,7 +6895,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="97" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>159</v>
       </c>
@@ -6954,7 +6954,7 @@
         <v>0.13763186899999999</v>
       </c>
     </row>
-    <row r="98" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>159</v>
       </c>
@@ -7013,7 +7013,7 @@
         <v>0.86236813099999998</v>
       </c>
     </row>
-    <row r="99" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>159</v>
       </c>
@@ -7072,7 +7072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>165</v>
       </c>
@@ -7131,7 +7131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>165</v>
       </c>
@@ -7190,7 +7190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>169</v>
       </c>
@@ -7249,7 +7249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>169</v>
       </c>
@@ -7308,7 +7308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>173</v>
       </c>
@@ -7367,7 +7367,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="105" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>173</v>
       </c>
@@ -7426,7 +7426,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="106" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>173</v>
       </c>
@@ -7485,7 +7485,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="107" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>173</v>
       </c>
@@ -7544,7 +7544,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="108" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>174</v>
       </c>
@@ -7603,7 +7603,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="109" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>174</v>
       </c>
@@ -7662,7 +7662,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="110" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>174</v>
       </c>
@@ -7721,7 +7721,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="111" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>176</v>
       </c>
@@ -7780,7 +7780,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="112" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>176</v>
       </c>
@@ -7839,7 +7839,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="113" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>176</v>
       </c>
@@ -7898,7 +7898,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="114" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>177</v>
       </c>
@@ -7957,7 +7957,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="115" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>177</v>
       </c>
@@ -8016,7 +8016,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="116" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>177</v>
       </c>
@@ -8075,7 +8075,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="117" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>178</v>
       </c>
@@ -8134,7 +8134,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="118" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>179</v>
       </c>
@@ -8193,7 +8193,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="119" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>180</v>
       </c>
@@ -8252,7 +8252,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="120" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>181</v>
       </c>
@@ -8311,7 +8311,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="121" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>182</v>
       </c>
@@ -8370,7 +8370,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="122" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>183</v>
       </c>
@@ -8429,7 +8429,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="123" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>184</v>
       </c>
@@ -8488,7 +8488,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="124" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>185</v>
       </c>
@@ -8547,7 +8547,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="125" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>186</v>
       </c>
@@ -8606,7 +8606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>190</v>
       </c>
@@ -8665,7 +8665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>193</v>
       </c>
@@ -8724,7 +8724,7 @@
         <v>1.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="128" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>193</v>
       </c>
@@ -8783,7 +8783,7 @@
         <v>1.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="129" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>193</v>
       </c>
@@ -8842,7 +8842,7 @@
         <v>1.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="130" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>193</v>
       </c>
@@ -8901,7 +8901,7 @@
         <v>1.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>193</v>
       </c>
@@ -8960,7 +8960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>193</v>
       </c>
@@ -9019,7 +9019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>198</v>
       </c>
@@ -9078,7 +9078,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="134" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>198</v>
       </c>
@@ -9137,7 +9137,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="135" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>198</v>
       </c>
@@ -9196,7 +9196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>199</v>
       </c>
@@ -9255,7 +9255,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="137" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>199</v>
       </c>
@@ -9314,7 +9314,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="138" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>200</v>
       </c>
@@ -9373,7 +9373,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="139" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>200</v>
       </c>
@@ -9432,7 +9432,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="140" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>201</v>
       </c>
@@ -9491,7 +9491,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="141" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>201</v>
       </c>
@@ -9550,7 +9550,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="142" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>201</v>
       </c>
@@ -9609,7 +9609,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="143" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>202</v>
       </c>
@@ -9668,7 +9668,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="144" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>202</v>
       </c>
@@ -9727,7 +9727,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="145" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>202</v>
       </c>
@@ -9786,7 +9786,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="146" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>203</v>
       </c>
@@ -9845,7 +9845,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="147" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>204</v>
       </c>
@@ -9904,7 +9904,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="148" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>205</v>
       </c>
@@ -9963,7 +9963,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="149" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>206</v>
       </c>
@@ -10022,7 +10022,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="150" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>207</v>
       </c>
@@ -10081,7 +10081,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="151" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>208</v>
       </c>
@@ -10140,7 +10140,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="152" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>209</v>
       </c>
@@ -10199,7 +10199,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="153" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>210</v>
       </c>
@@ -10258,7 +10258,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="154" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>210</v>
       </c>
@@ -10317,7 +10317,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="155" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>212</v>
       </c>
@@ -10376,7 +10376,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="156" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>212</v>
       </c>
@@ -10435,7 +10435,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="157" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>213</v>
       </c>
@@ -10494,7 +10494,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="158" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>217</v>
       </c>
@@ -10553,7 +10553,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="159" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>220</v>
       </c>
@@ -10612,7 +10612,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="160" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>222</v>
       </c>
@@ -10671,7 +10671,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="161" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>222</v>
       </c>
@@ -10730,7 +10730,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="162" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>225</v>
       </c>
@@ -10789,7 +10789,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="163" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>225</v>
       </c>
@@ -10848,7 +10848,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="164" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>228</v>
       </c>
@@ -10907,7 +10907,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="165" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>229</v>
       </c>
@@ -10966,7 +10966,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="166" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>229</v>
       </c>
@@ -11025,7 +11025,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="167" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>229</v>
       </c>
@@ -11084,7 +11084,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="168" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>230</v>
       </c>
@@ -11143,7 +11143,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="169" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>230</v>
       </c>
@@ -11202,7 +11202,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="170" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>231</v>
       </c>
@@ -11261,7 +11261,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="171" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>231</v>
       </c>
@@ -11320,7 +11320,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="172" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>231</v>
       </c>
@@ -11379,7 +11379,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="173" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>232</v>
       </c>
@@ -11438,7 +11438,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="174" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>232</v>
       </c>
@@ -11497,7 +11497,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="175" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>232</v>
       </c>
@@ -11556,7 +11556,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="176" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>233</v>
       </c>
@@ -11615,7 +11615,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="177" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>234</v>
       </c>
@@ -11674,7 +11674,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="178" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>235</v>
       </c>
@@ -11733,7 +11733,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="179" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>236</v>
       </c>
@@ -11792,7 +11792,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="180" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>237</v>
       </c>
@@ -11851,7 +11851,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="181" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>238</v>
       </c>
@@ -11910,7 +11910,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="182" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>239</v>
       </c>
@@ -11969,7 +11969,7 @@
         <v>0.90500000000000003</v>
       </c>
     </row>
-    <row r="183" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>239</v>
       </c>
@@ -12028,7 +12028,7 @@
         <v>0.89500000000000002</v>
       </c>
     </row>
-    <row r="184" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>239</v>
       </c>
@@ -12087,7 +12087,7 @@
         <v>0.105</v>
       </c>
     </row>
-    <row r="185" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>239</v>
       </c>
@@ -12146,7 +12146,7 @@
         <v>9.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="186" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>241</v>
       </c>
@@ -12205,7 +12205,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="187" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>241</v>
       </c>
@@ -12264,7 +12264,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="188" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>241</v>
       </c>
@@ -12323,7 +12323,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="189" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>241</v>
       </c>
@@ -12382,7 +12382,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="190" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>243</v>
       </c>
@@ -12441,7 +12441,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="191" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>243</v>
       </c>
@@ -12500,7 +12500,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="192" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>243</v>
       </c>
@@ -12559,7 +12559,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="193" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>243</v>
       </c>
@@ -12618,7 +12618,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="194" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>244</v>
       </c>
@@ -12677,7 +12677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>247</v>
       </c>
@@ -12736,7 +12736,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="196" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>247</v>
       </c>
@@ -12795,7 +12795,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="197" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>249</v>
       </c>
@@ -12854,7 +12854,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="198" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>251</v>
       </c>
@@ -12913,7 +12913,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="199" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>251</v>
       </c>
@@ -12972,7 +12972,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="200" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>251</v>
       </c>
@@ -13031,7 +13031,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="201" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>251</v>
       </c>
@@ -13090,7 +13090,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="202" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>256</v>
       </c>
@@ -13149,7 +13149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>259</v>
       </c>
@@ -13208,7 +13208,7 @@
         <v>0.91214953271027999</v>
       </c>
     </row>
-    <row r="204" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>259</v>
       </c>
@@ -13267,7 +13267,7 @@
         <v>0.91214953271027999</v>
       </c>
     </row>
-    <row r="205" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>259</v>
       </c>
@@ -13326,7 +13326,7 @@
         <v>8.7850467289719597E-2</v>
       </c>
     </row>
-    <row r="206" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>259</v>
       </c>
@@ -13385,7 +13385,7 @@
         <v>8.7850467289719597E-2</v>
       </c>
     </row>
-    <row r="207" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>264</v>
       </c>
@@ -13444,7 +13444,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="208" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>268</v>
       </c>
@@ -13503,7 +13503,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="209" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>272</v>
       </c>
@@ -13562,7 +13562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>275</v>
       </c>
@@ -13621,7 +13621,7 @@
         <v>2.7E-2</v>
       </c>
     </row>
-    <row r="211" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>275</v>
       </c>
@@ -13680,7 +13680,7 @@
         <v>2.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="212" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>277</v>
       </c>
@@ -13749,7 +13749,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="213" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>277</v>
       </c>
@@ -13818,7 +13818,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="214" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>277</v>
       </c>
@@ -13887,7 +13887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>277</v>
       </c>
@@ -13956,7 +13956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>282</v>
       </c>

</xml_diff>